<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-study-summary-ig@09c793aead3c2177e4622c9d4cf0f19a3da98b0d 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-study-dd-table.xlsx
+++ b/StructureDefinition-study-dd-table.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-22T15:57:32+00:00</t>
+    <t>2022-04-26T17:19:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>82</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-study-summary-ig@8df1ac84bdce05f1e547c4a31afd2f21af12eaa0 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-study-dd-table.xlsx
+++ b/StructureDefinition-study-dd-table.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-26T17:20:41+00:00</t>
+    <t>2022-04-26T22:45:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>82</v>

</xml_diff>